<commit_message>
sort the words by dic
</commit_message>
<xml_diff>
--- a/verbs.xlsx
+++ b/verbs.xlsx
@@ -588,15 +588,17 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="9.875" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="10.875" customWidth="1"/>
+    <col min="1" max="1" width="13.75" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="15.375" customWidth="1"/>
+    <col min="4" max="4" width="12.625" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="13.125" customWidth="1"/>
     <col min="7" max="7" width="24.625" customWidth="1"/>
     <col min="8" max="8" width="27" customWidth="1"/>
     <col min="9" max="9" width="32.25" customWidth="1"/>
@@ -635,25 +637,25 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
@@ -681,112 +683,115 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="27" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="G6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G7" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="G8" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A3:I8">
+    <sortCondition ref="D3:D8"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>